<commit_message>
mejoras descriptive en ingles
</commit_message>
<xml_diff>
--- a/articulo 1 XAI/Data_example/data_descriptive.xlsx
+++ b/articulo 1 XAI/Data_example/data_descriptive.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Doctorado EOMA\Cafee\articulo 1 XAI\Data_example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://miumh-my.sharepoint.com/personal/ricardo_gonzalezm_miumh_umh_es/Documents/Documentos/Cafee/articulo 1 XAI/Data_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B8FB5D-AB88-4690-A9D5-1358A29A722A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{29B8FB5D-AB88-4690-A9D5-1358A29A722A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D26669A-0A36-45BA-8627-E67D32FAB565}"/>
   <bookViews>
-    <workbookView xWindow="1509" yWindow="1509" windowWidth="21574" windowHeight="10894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2340" yWindow="600" windowWidth="21600" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>(1,09)</t>
   </si>
   <si>
-    <t>Andalucia</t>
-  </si>
-  <si>
     <t>Aragon</t>
   </si>
   <si>
@@ -364,12 +361,6 @@
     <t>La Rioja</t>
   </si>
   <si>
-    <t>Madrid</t>
-  </si>
-  <si>
-    <t>Murcia</t>
-  </si>
-  <si>
     <t>Navarre</t>
   </si>
   <si>
@@ -377,6 +368,15 @@
   </si>
   <si>
     <t>Valencian Community</t>
+  </si>
+  <si>
+    <t>Andalusia</t>
+  </si>
+  <si>
+    <t>Community of Madrid</t>
+  </si>
+  <si>
+    <t>Region of Murcia</t>
   </si>
 </sst>
 </file>
@@ -687,19 +687,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1000,43 +1000,43 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:R18"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A1" s="19"/>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="18"/>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15" t="s">
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="15"/>
+      <c r="N1" s="19"/>
       <c r="O1" s="5" t="s">
         <v>2</v>
       </c>
@@ -1050,12 +1050,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="16">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="C2" s="13">
         <v>469.44799999999998</v>
@@ -1106,12 +1106,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="17">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="13">
         <v>493.10899999999998</v>
@@ -1162,12 +1162,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="17">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="13">
         <v>496.10500000000002</v>
@@ -1218,12 +1218,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="17">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="13">
         <v>481.142</v>
@@ -1274,12 +1274,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="17">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="13">
         <v>468.78500000000003</v>
@@ -1330,12 +1330,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="17">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="13">
         <v>494.084</v>
@@ -1386,12 +1386,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="17">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="13">
         <v>499.803</v>
@@ -1442,12 +1442,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="17">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="13">
         <v>485.28899999999999</v>
@@ -1498,12 +1498,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="17">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="13">
         <v>487.096</v>
@@ -1554,12 +1554,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="17">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="13">
         <v>472.57499999999999</v>
@@ -1610,12 +1610,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A12" s="17">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="13">
         <v>510.166</v>
@@ -1666,12 +1666,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="17">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="13">
         <v>481.82600000000002</v>
@@ -1722,12 +1722,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="17">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C14" s="13">
         <v>495.18099999999998</v>
@@ -1778,12 +1778,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="17">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C15" s="13">
         <v>480.63499999999999</v>
@@ -1834,12 +1834,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="17">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C16" s="13">
         <v>492.91199999999998</v>
@@ -1890,12 +1890,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="17">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" s="13">
         <v>481.95699999999999</v>
@@ -1946,12 +1946,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="18">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C18" s="14">
         <v>479.33100000000002</v>

</xml_diff>